<commit_message>
updated line of augmentation (needs to be completed)
</commit_message>
<xml_diff>
--- a/e2e.xlsx
+++ b/e2e.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulia Ciaramella\PycharmProjects\yolov5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB4363E-7FF6-4D2B-BEC7-CB57362937F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D445ECB7-D531-4947-BF57-D6E0EEA5CCDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EAF970FA-349E-491A-84BE-B32BF07A602C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>STEP</t>
   </si>
@@ -580,6 +580,46 @@
   </si>
   <si>
     <t xml:space="preserve">so far, the best model was reached by selecting: 100 epochs, 64 batches and image size of 640*640px </t>
+  </si>
+  <si>
+    <t>augmentation is done only on training data. The transformation applied are: ____________</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">after each transformation, a copy of the image is saved. If gray scale is applied, the image will be called: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>original_name_gray.png</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Then the  program copies the txt file of the original images but the name of the txt becomes: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>original_name_gray.txt</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1285,14 +1325,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B1BCCE-6C46-484C-8C13-A38ED5FE04C3}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="120" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="25.7109375" style="1"/>
-    <col min="3" max="3" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="50.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="44.5703125" style="1" customWidth="1"/>
@@ -1437,8 +1477,15 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>